<commit_message>
Column Wise analysis and MetaData
</commit_message>
<xml_diff>
--- a/metadata_Observation.xlsx
+++ b/metadata_Observation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="154">
   <si>
     <t>id</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>array(['B', 'C', 'A', 'E', 'F', 'D', 'G']</t>
-  </si>
-  <si>
-    <t>3 Records with NONE</t>
   </si>
   <si>
     <t>* More the Annual Income More the Intereset Rate
@@ -280,13 +277,7 @@
     <t>array(['Fully Paid', 'Charged Off', 'Current']</t>
   </si>
   <si>
-    <t>Just Single Unique Record, Can be Discarded</t>
-  </si>
-  <si>
     <t>Same as MemberID, Can be Discarded</t>
-  </si>
-  <si>
-    <t>Can be checked later if any texts are useful</t>
   </si>
   <si>
     <t>array(['credit_card', 'car', 'small_business', 'other', 'wedding',
@@ -318,9 +309,6 @@
 This is the sequence of Loan Amount in Ascending Order</t>
   </si>
   <si>
-    <t>Can Checked Later if any texts are useful</t>
-  </si>
-  <si>
     <t>* Not Able to See Any Corelated Columns</t>
   </si>
   <si>
@@ -366,9 +354,6 @@
   </si>
   <si>
     <t>* Total credit revolving balance</t>
-  </si>
-  <si>
-    <t>* Revolving line utilization rate, or the amount of credit the borrower is using relative to all available revolving credit.</t>
   </si>
   <si>
     <t>0    83.70%
@@ -389,9 +374,6 @@
     <t>Unique Values/Head()</t>
   </si>
   <si>
-    <t>* One Unique Value can be Drop this Column</t>
-  </si>
-  <si>
     <t>* Remaining outstanding principal for total amount funded</t>
   </si>
   <si>
@@ -434,23 +416,184 @@
     <t>* Number of collections in 12 months excluding medical collections</t>
   </si>
   <si>
-    <t>* The number of accounts on which the borrower is now delinquent.</t>
-  </si>
-  <si>
-    <t>* The past-due amount owed for the accounts on which the borrower is now delinquent.</t>
-  </si>
-  <si>
     <t>* Number of public record bankruptcies</t>
   </si>
   <si>
     <t>Category &gt; 0 and 0</t>
+  </si>
+  <si>
+    <t>* The total number of credit lines currently in the borrower's credit file</t>
+  </si>
+  <si>
+    <t>Can be Catagorical</t>
+  </si>
+  <si>
+    <t>Date Based Category</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>array(['0', nan]</t>
+  </si>
+  <si>
+    <t>array([nan, 'Jun-16', 'Jul-16']</t>
+  </si>
+  <si>
+    <t>array(['1'], dtype=object)</t>
+  </si>
+  <si>
+    <t>* Can be Dropped</t>
+  </si>
+  <si>
+    <t>array(['INDIVIDUAL'], dtype=object)</t>
+  </si>
+  <si>
+    <t>array(['0'], dtype=object)</t>
+  </si>
+  <si>
+    <t>* The number of accounts on which the borrower is now delinquent.
+* Can be Dropped</t>
+  </si>
+  <si>
+    <t>array(['0', nan], dtype=object)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* The past-due amount owed for the accounts on which the borrower is now delinquent.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Can be Dropped</t>
+    </r>
+  </si>
+  <si>
+    <t>array(['0', '1', '2', nan], dtype=object)</t>
+  </si>
+  <si>
+    <t>* Number of tax liens</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Can be checked later if any texts are useful
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Can be Dropped</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Can Checked Later if any texts are useful
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Can be Dropped</t>
+    </r>
+  </si>
+  <si>
+    <t>array(['f'], dtype=object)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* One Unique Value can be Drop this Column
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Can be Dropped</t>
+    </r>
+  </si>
+  <si>
+    <t>array(['n'], dtype=object)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just Single Unique Record, Can be Discarded
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* Can be Dropped</t>
+    </r>
+  </si>
+  <si>
+    <t>Categorical Based on Other Data</t>
+  </si>
+  <si>
+    <t>3 Records with NONE, With "Full Paid" Category</t>
+  </si>
+  <si>
+    <t>25682 (64%)</t>
+  </si>
+  <si>
+    <t>36931(92%)</t>
+  </si>
+  <si>
+    <t>* Revolving line utilization rate, or the amount of credit the borrower is using relative to all available revolving credit.
+* Need to Check about the NAN Value Filling Part.</t>
+  </si>
+  <si>
+    <t>16 NULL for ChargeOff Scenario</t>
+  </si>
+  <si>
+    <t>0        May-16
+1        Sep-13
+2        May-16
+3        Apr-16
+4        May-16
+5        Jan-16
+6        May-16
+7        Dec-14
+8        Aug-12
+9        Mar-13
+10       Dec-15</t>
+  </si>
+  <si>
+    <t>14% Null Value</t>
+  </si>
+  <si>
+    <t>* Need to Check for NAN Value Update</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +638,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -523,13 +672,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -588,7 +737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -614,7 +763,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
@@ -1107,17 +1262,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="C62" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="11" customWidth="1"/>
@@ -1183,7 +1338,7 @@
         <v>77</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="I10" t="s">
         <v>66</v>
@@ -1408,15 +1563,21 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1">
+        <v>2459</v>
+      </c>
       <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="I21" s="16" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="30">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
         <v>12</v>
@@ -1433,7 +1594,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" ht="45">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1444,8 +1605,8 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
-        <v>82</v>
+      <c r="G23" s="8" t="s">
+        <v>146</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>79</v>
@@ -1466,7 +1627,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30">
@@ -1482,7 +1643,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I25" s="8"/>
     </row>
@@ -1500,7 +1661,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1516,11 +1677,11 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I27" s="8"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" ht="30">
       <c r="A28" s="5" t="s">
         <v>17</v>
       </c>
@@ -1532,9 +1693,11 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="8"/>
+      <c r="H28" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="I28" s="8" t="s">
-        <v>87</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1549,11 +1712,11 @@
       <c r="G29" s="1"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30">
+      <c r="A30" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="1"/>
@@ -1564,11 +1727,11 @@
       <c r="G30" s="1"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="240">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B31" s="1"/>
@@ -1577,21 +1740,21 @@
         <v>14</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I31" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="14" t="s">
+    </row>
+    <row r="32" spans="1:9" ht="30">
+      <c r="A32" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="1"/>
@@ -1604,7 +1767,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1623,7 +1786,7 @@
       <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B34" s="1"/>
@@ -1636,11 +1799,11 @@
       <c r="G34" s="1"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="75">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B35" s="1"/>
@@ -1652,10 +1815,10 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30">
@@ -1671,10 +1834,10 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1705,18 +1868,18 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="45">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>102</v>
+      <c r="B39" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1">
@@ -1724,16 +1887,16 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="1">
-        <v>25682</v>
+      <c r="G39" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="H39" s="8"/>
       <c r="I39" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B40" s="1"/>
@@ -1743,8 +1906,8 @@
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="1">
-        <v>36931</v>
+      <c r="G40" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
@@ -1762,10 +1925,10 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1781,10 +1944,10 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1792,7 +1955,7 @@
         <v>32</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1">
@@ -1803,7 +1966,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="75">
@@ -1817,32 +1980,40 @@
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="G44" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="H44" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="90">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1">
         <v>82</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
       <c r="H45" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I45" s="8"/>
-    </row>
-    <row r="46" spans="1:9">
+        <v>106</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30">
       <c r="A46" s="13" t="s">
         <v>35</v>
       </c>
@@ -1854,9 +2025,11 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="8"/>
+      <c r="H46" s="8" t="s">
+        <v>141</v>
+      </c>
       <c r="I46" s="8" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="30">
@@ -1864,7 +2037,7 @@
         <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1">
@@ -1875,7 +2048,7 @@
       <c r="G47" s="1"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="30">
@@ -1883,7 +2056,7 @@
         <v>37</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
@@ -1894,7 +2067,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30">
@@ -1902,16 +2075,18 @@
         <v>38</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1">
+        <v>37850</v>
+      </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="30">
@@ -1919,16 +2094,18 @@
         <v>39</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
+      <c r="D50" s="1">
+        <v>37850</v>
+      </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1936,16 +2113,18 @@
         <v>40</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="D51" s="1">
+        <v>7976</v>
+      </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1953,87 +2132,103 @@
         <v>41</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
+      <c r="D52" s="1">
+        <v>35148</v>
+      </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
+      <c r="D53" s="1">
+        <v>1356</v>
+      </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="15" t="s">
         <v>43</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
+      <c r="D54" s="1">
+        <v>4040</v>
+      </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
+      <c r="D55" s="1">
+        <v>2616</v>
+      </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="8"/>
       <c r="I55" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
+      <c r="D56" s="1">
+        <v>102</v>
+      </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2043,146 +2238,208 @@
       <c r="I57" s="8"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B58" s="1"/>
+      <c r="B58" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
+      <c r="D58" s="1">
+        <v>3</v>
+      </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-      <c r="H58" s="8"/>
+      <c r="H58" s="8" t="s">
+        <v>129</v>
+      </c>
       <c r="I58" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="30">
-      <c r="A59" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="165">
+      <c r="A59" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B59" s="1"/>
+      <c r="B59" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="D59" s="1">
+        <v>107</v>
+      </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="8"/>
+      <c r="H59" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="I59" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="30">
       <c r="A60" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
+      <c r="D60" s="1">
+        <v>2</v>
+      </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
-      <c r="H60" s="8"/>
+      <c r="H60" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="I60" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="13" t="s">
         <v>50</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
+      <c r="H61" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I61" s="16" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-    </row>
-    <row r="63" spans="1:9" ht="30">
-      <c r="A63" s="1" t="s">
+      <c r="H62" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="I62" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="45">
+      <c r="A63" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
+      <c r="D63" s="1">
+        <v>1</v>
+      </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-      <c r="H63" s="8"/>
+      <c r="H63" s="8" t="s">
+        <v>133</v>
+      </c>
       <c r="I63" s="8" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
+      <c r="D64" s="1">
+        <v>2</v>
+      </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-    </row>
-    <row r="65" spans="1:9" ht="30">
-      <c r="A65" s="1" t="s">
+      <c r="G64" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I64" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="45">
+      <c r="A65" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
+      <c r="D65" s="1">
+        <v>1</v>
+      </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-      <c r="H65" s="8"/>
+      <c r="H65" s="8" t="s">
+        <v>133</v>
+      </c>
       <c r="I65" s="8" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B66" s="1"/>
+      <c r="B66" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="D66" s="1">
+        <v>4</v>
+      </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-      <c r="H66" s="8"/>
+      <c r="H66" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="I66" s="8" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B67" s="2"/>
+      <c r="B67" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+      <c r="D67" s="2">
+        <v>2</v>
+      </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="10"/>
-      <c r="I67" s="10"/>
+      <c r="H67" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>